<commit_message>
Updated Global_M2 for easier usage.
</commit_message>
<xml_diff>
--- a/Global_M2/TVDataFeed/FinalData/Argentina.xlsx
+++ b/Global_M2/TVDataFeed/FinalData/Argentina.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D398"/>
+  <dimension ref="A1:D401"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5449,13 +5449,13 @@
         <v>44621</v>
       </c>
       <c r="B388" t="n">
-        <v>7431016000000</v>
+        <v>7431065591000</v>
       </c>
       <c r="C388" t="n">
         <v>0.009009009009009009</v>
       </c>
       <c r="D388" t="n">
-        <v>66946090090.09009</v>
+        <v>66946536855.85586</v>
       </c>
     </row>
     <row r="389">
@@ -5463,13 +5463,13 @@
         <v>44652</v>
       </c>
       <c r="B389" t="n">
-        <v>7779471500000</v>
+        <v>7779488501000</v>
       </c>
       <c r="C389" t="n">
         <v>0.008672274737663689</v>
       </c>
       <c r="D389" t="n">
-        <v>67465714161.82465</v>
+        <v>67465861599.16747</v>
       </c>
     </row>
     <row r="390">
@@ -5477,13 +5477,13 @@
         <v>44682</v>
       </c>
       <c r="B390" t="n">
-        <v>8162697100000</v>
+        <v>8162661859000</v>
       </c>
       <c r="C390" t="n">
         <v>0.008320159747067143</v>
       </c>
       <c r="D390" t="n">
-        <v>67914943838.9217</v>
+        <v>67914650628.17206</v>
       </c>
     </row>
     <row r="391">
@@ -5596,6 +5596,48 @@
       </c>
       <c r="D398" t="n">
         <v>68300797946.30442</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="2" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B399" t="n">
+        <v>13551717200000</v>
+      </c>
+      <c r="C399" t="n">
+        <v>0.00507227998985544</v>
+      </c>
+      <c r="D399" t="n">
+        <v>68738103981.73979</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="2" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B400" t="n">
+        <v>13436944380000</v>
+      </c>
+      <c r="C400" t="n">
+        <v>0.004785146904009953</v>
+      </c>
+      <c r="D400" t="n">
+        <v>64297752799.31094</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="2" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B401" t="n">
+        <v>14573629300000</v>
+      </c>
+      <c r="C401" t="n">
+        <v>0.004491555874955084</v>
+      </c>
+      <c r="D401" t="n">
+        <v>65458270301.83256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>